<commit_message>
Add more penetrable brick
</commit_message>
<xml_diff>
--- a/Enemies.xlsx
+++ b/Enemies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pacif\Desktop\nhapmongame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBDF08D-74C8-4FBF-836B-751AD942A693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7311F525-05F3-44A4-BDF4-B27A04AE5E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-290" yWindow="740" windowWidth="13870" windowHeight="9170" activeTab="3" xr2:uid="{3CE8D76A-6137-4DED-8FB9-A002D5CB39E0}"/>
+    <workbookView xWindow="5060" yWindow="1030" windowWidth="13870" windowHeight="9170" activeTab="3" xr2:uid="{3CE8D76A-6137-4DED-8FB9-A002D5CB39E0}"/>
   </bookViews>
   <sheets>
     <sheet name="sprite" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="68">
   <si>
     <t>enemy1</t>
   </si>
@@ -154,6 +154,93 @@
   </si>
   <si>
     <t>enemy10</t>
+  </si>
+  <si>
+    <t>Enemy bullet</t>
+  </si>
+  <si>
+    <t>Enemy11 (màu hồng)</t>
+  </si>
+  <si>
+    <t>Enemy12 (màu đen)</t>
+  </si>
+  <si>
+    <t>Enemy13 (eye)</t>
+  </si>
+  <si>
+    <t>Bình xăng có đạn</t>
+  </si>
+  <si>
+    <t>Xăng item</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>E7</t>
+  </si>
+  <si>
+    <t>E8</t>
+  </si>
+  <si>
+    <t>E9</t>
+  </si>
+  <si>
+    <t>E10</t>
+  </si>
+  <si>
+    <t>Bullet2</t>
+  </si>
+  <si>
+    <t>Enemy11 (màu hồng, zic zac Y)</t>
+  </si>
+  <si>
+    <t>Enemy12 (màu đen, ziczac x)</t>
+  </si>
+  <si>
+    <t>Màu hồng, ziczac X</t>
+  </si>
+  <si>
+    <t>(màu đen, ziczac x)</t>
+  </si>
+  <si>
+    <t>ĐI lung tung, bắn đạn</t>
+  </si>
+  <si>
+    <t>Đen, đi ngang</t>
+  </si>
+  <si>
+    <t>(màu hồng, zic zac Y)</t>
+  </si>
+  <si>
+    <t>Hồng, ngang</t>
+  </si>
+  <si>
+    <t>Hồng, đi tới Jason</t>
+  </si>
+  <si>
+    <t>Enemy13 (eye), đi ngang</t>
+  </si>
+  <si>
+    <t>(màu đen, ziczac y)</t>
   </si>
 </sst>
 </file>
@@ -511,13 +598,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E190BF18-1A6B-4524-A793-DF9DF2FA9D0D}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28:G28"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G29" sqref="A29:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.7265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
@@ -610,7 +700,7 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B28" si="0">B3+1</f>
+        <f t="shared" ref="B4:B47" si="0">B3+1</f>
         <v>8002</v>
       </c>
       <c r="C4">
@@ -1084,7 +1174,7 @@
         <v>37</v>
       </c>
       <c r="E20">
-        <f t="shared" ref="E20:E21" si="10">C20+18</f>
+        <f t="shared" ref="E20" si="10">C20+18</f>
         <v>210</v>
       </c>
       <c r="F20">
@@ -1204,6 +1294,9 @@
       <c r="G24">
         <v>50</v>
       </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B25">
@@ -1227,6 +1320,9 @@
       <c r="G25">
         <v>50</v>
       </c>
+      <c r="H25">
+        <v>2</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B26">
@@ -1250,6 +1346,9 @@
       <c r="G26">
         <v>50</v>
       </c>
+      <c r="H26">
+        <v>2</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B27">
@@ -1273,6 +1372,9 @@
       <c r="G27">
         <v>50</v>
       </c>
+      <c r="H27">
+        <v>2</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
@@ -1298,6 +1400,419 @@
       </c>
       <c r="G28">
         <v>50</v>
+      </c>
+      <c r="H28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>8027</v>
+      </c>
+      <c r="C29">
+        <v>214</v>
+      </c>
+      <c r="D29">
+        <v>1159</v>
+      </c>
+      <c r="E29">
+        <f>8+C29</f>
+        <v>222</v>
+      </c>
+      <c r="F29">
+        <f>8+D29</f>
+        <v>1167</v>
+      </c>
+      <c r="G29">
+        <v>50</v>
+      </c>
+      <c r="H29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>8028</v>
+      </c>
+      <c r="C30">
+        <v>84</v>
+      </c>
+      <c r="D30">
+        <v>1150</v>
+      </c>
+      <c r="E30">
+        <f>C30+18</f>
+        <v>102</v>
+      </c>
+      <c r="F30">
+        <f>D30+17</f>
+        <v>1167</v>
+      </c>
+      <c r="H30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>8029</v>
+      </c>
+      <c r="C31">
+        <v>104</v>
+      </c>
+      <c r="D31">
+        <v>1151</v>
+      </c>
+      <c r="E31">
+        <f>C31+18</f>
+        <v>122</v>
+      </c>
+      <c r="F31">
+        <f>D31+16</f>
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>8030</v>
+      </c>
+      <c r="C32">
+        <v>132</v>
+      </c>
+      <c r="D32">
+        <v>1151</v>
+      </c>
+      <c r="E32">
+        <f>C32+18</f>
+        <v>150</v>
+      </c>
+      <c r="F32">
+        <f>D32+16</f>
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>8031</v>
+      </c>
+      <c r="C33">
+        <v>152</v>
+      </c>
+      <c r="D33">
+        <v>1150</v>
+      </c>
+      <c r="E33">
+        <f>C33+18</f>
+        <v>170</v>
+      </c>
+      <c r="F33">
+        <f>D33+17</f>
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>8032</v>
+      </c>
+      <c r="C34">
+        <v>84</v>
+      </c>
+      <c r="D34">
+        <v>296</v>
+      </c>
+      <c r="E34">
+        <f>C34+18</f>
+        <v>102</v>
+      </c>
+      <c r="F34">
+        <f>D34+17</f>
+        <v>313</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>8033</v>
+      </c>
+      <c r="C35">
+        <v>104</v>
+      </c>
+      <c r="D35">
+        <v>297</v>
+      </c>
+      <c r="E35">
+        <f>C35+18</f>
+        <v>122</v>
+      </c>
+      <c r="F35">
+        <f>D35+16</f>
+        <v>313</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>8034</v>
+      </c>
+      <c r="C36">
+        <v>132</v>
+      </c>
+      <c r="D36">
+        <v>296</v>
+      </c>
+      <c r="E36">
+        <f>C36+18</f>
+        <v>150</v>
+      </c>
+      <c r="F36">
+        <f>D36+16</f>
+        <v>312</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>8035</v>
+      </c>
+      <c r="C37">
+        <v>152</v>
+      </c>
+      <c r="D37">
+        <v>297</v>
+      </c>
+      <c r="E37">
+        <f>C37+18</f>
+        <v>170</v>
+      </c>
+      <c r="F37">
+        <f>D37+17</f>
+        <v>314</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>8036</v>
+      </c>
+      <c r="C38">
+        <v>44</v>
+      </c>
+      <c r="D38">
+        <v>217</v>
+      </c>
+      <c r="E38">
+        <f>C38+18</f>
+        <v>62</v>
+      </c>
+      <c r="F38">
+        <f>D38+16</f>
+        <v>233</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>8037</v>
+      </c>
+      <c r="C39">
+        <v>64</v>
+      </c>
+      <c r="D39">
+        <v>275</v>
+      </c>
+      <c r="E39">
+        <f>C39+18</f>
+        <v>82</v>
+      </c>
+      <c r="F39">
+        <f>D39+18</f>
+        <v>293</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>8038</v>
+      </c>
+      <c r="C40">
+        <v>84</v>
+      </c>
+      <c r="D40">
+        <v>277</v>
+      </c>
+      <c r="E40">
+        <f>C40+18</f>
+        <v>102</v>
+      </c>
+      <c r="F40">
+        <f>D40+16</f>
+        <v>293</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>8039</v>
+      </c>
+      <c r="C41">
+        <v>104</v>
+      </c>
+      <c r="D41">
+        <v>275</v>
+      </c>
+      <c r="E41">
+        <f>C41+18</f>
+        <v>122</v>
+      </c>
+      <c r="F41">
+        <f>D41+18</f>
+        <v>293</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>8040</v>
+      </c>
+      <c r="C42">
+        <v>132</v>
+      </c>
+      <c r="D42">
+        <v>718</v>
+      </c>
+      <c r="E42">
+        <f>C42+17</f>
+        <v>149</v>
+      </c>
+      <c r="F42">
+        <f>D42+18</f>
+        <v>736</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>8041</v>
+      </c>
+      <c r="C43">
+        <v>150</v>
+      </c>
+      <c r="D43">
+        <v>718</v>
+      </c>
+      <c r="E43">
+        <f>C43+17</f>
+        <v>167</v>
+      </c>
+      <c r="F43">
+        <f>D43+18</f>
+        <v>736</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="0"/>
+        <v>8042</v>
+      </c>
+      <c r="C44">
+        <v>5</v>
+      </c>
+      <c r="D44">
+        <v>59</v>
+      </c>
+      <c r="E44">
+        <f>C44+16</f>
+        <v>21</v>
+      </c>
+      <c r="F44">
+        <f>D44+16</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="0"/>
+        <v>8043</v>
+      </c>
+      <c r="C45">
+        <v>204</v>
+      </c>
+      <c r="D45">
+        <v>158</v>
+      </c>
+      <c r="E45">
+        <f>C45+18</f>
+        <v>222</v>
+      </c>
+      <c r="F45">
+        <f>D45+18</f>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B46">
+        <f t="shared" si="0"/>
+        <v>8044</v>
+      </c>
+      <c r="C46">
+        <v>254</v>
+      </c>
+      <c r="D46">
+        <v>158</v>
+      </c>
+      <c r="E46">
+        <f>C46+18</f>
+        <v>272</v>
+      </c>
+      <c r="F46">
+        <f>D46+18</f>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B47">
+        <f t="shared" si="0"/>
+        <v>8045</v>
+      </c>
+      <c r="C47">
+        <v>304</v>
+      </c>
+      <c r="D47">
+        <v>158</v>
+      </c>
+      <c r="E47">
+        <f>C47+18</f>
+        <v>322</v>
+      </c>
+      <c r="F47">
+        <f>D47+18</f>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -1308,269 +1823,480 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A6AB9CF-1CAF-4D10-99CD-3D53CBA5FD07}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2">
         <v>9100</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>8000</v>
       </c>
-      <c r="C2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <f t="shared" ref="A3:A11" si="0">A2+1</f>
+      <c r="D2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B19" si="0">B2+1</f>
         <v>9101</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>8001</v>
       </c>
-      <c r="C3">
-        <v>100</v>
-      </c>
       <c r="D3">
+        <v>100</v>
+      </c>
+      <c r="E3">
         <v>8002</v>
       </c>
-      <c r="E3">
-        <v>100</v>
-      </c>
       <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3">
         <v>8003</v>
       </c>
-      <c r="G3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="H3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4">
         <f t="shared" si="0"/>
         <v>9102</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>8004</v>
       </c>
-      <c r="C4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="D4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5">
         <f t="shared" si="0"/>
         <v>9103</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>8005</v>
       </c>
-      <c r="C5">
-        <v>100</v>
-      </c>
       <c r="D5">
+        <v>100</v>
+      </c>
+      <c r="E5">
         <v>8006</v>
       </c>
-      <c r="E5">
-        <v>100</v>
-      </c>
       <c r="F5">
+        <v>100</v>
+      </c>
+      <c r="G5">
         <v>8007</v>
       </c>
-      <c r="G5">
-        <v>100</v>
-      </c>
       <c r="H5">
+        <v>100</v>
+      </c>
+      <c r="I5">
         <v>8008</v>
       </c>
-      <c r="I5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="J5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6">
         <f t="shared" si="0"/>
         <v>9104</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>8009</v>
       </c>
-      <c r="C6">
-        <v>100</v>
-      </c>
       <c r="D6">
+        <v>100</v>
+      </c>
+      <c r="E6">
         <v>8010</v>
       </c>
-      <c r="E6">
-        <v>100</v>
-      </c>
       <c r="F6">
+        <v>100</v>
+      </c>
+      <c r="G6">
         <v>8011</v>
       </c>
-      <c r="G6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7">
+      <c r="H6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7">
         <f t="shared" si="0"/>
         <v>9105</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>8012</v>
       </c>
-      <c r="C7">
-        <v>100</v>
-      </c>
       <c r="D7">
+        <v>100</v>
+      </c>
+      <c r="E7">
         <v>8013</v>
       </c>
-      <c r="E7">
-        <v>100</v>
-      </c>
       <c r="F7">
+        <v>100</v>
+      </c>
+      <c r="G7">
         <v>8014</v>
       </c>
-      <c r="G7">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8">
+      <c r="H7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8">
         <f t="shared" si="0"/>
         <v>9106</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>8015</v>
       </c>
-      <c r="C8">
-        <v>100</v>
-      </c>
       <c r="D8">
+        <v>100</v>
+      </c>
+      <c r="E8">
         <v>8016</v>
       </c>
-      <c r="E8">
-        <v>100</v>
-      </c>
       <c r="F8">
+        <v>100</v>
+      </c>
+      <c r="G8">
         <v>8017</v>
       </c>
-      <c r="G8">
-        <v>100</v>
-      </c>
       <c r="H8">
+        <v>100</v>
+      </c>
+      <c r="I8">
         <v>8018</v>
       </c>
-      <c r="I8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9">
+      <c r="J8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9">
         <f t="shared" si="0"/>
         <v>9107</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>8019</v>
       </c>
-      <c r="C9">
-        <v>100</v>
-      </c>
       <c r="D9">
+        <v>100</v>
+      </c>
+      <c r="E9">
         <v>8020</v>
       </c>
-      <c r="E9">
-        <v>100</v>
-      </c>
       <c r="F9">
+        <v>100</v>
+      </c>
+      <c r="G9">
         <v>8021</v>
       </c>
-      <c r="G9">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10">
+      <c r="H9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10">
         <f t="shared" si="0"/>
         <v>9108</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>8022</v>
       </c>
-      <c r="C10">
-        <v>100</v>
-      </c>
       <c r="D10">
+        <v>100</v>
+      </c>
+      <c r="E10">
         <v>8023</v>
       </c>
-      <c r="E10">
-        <v>100</v>
-      </c>
       <c r="F10">
+        <v>100</v>
+      </c>
+      <c r="G10">
         <v>8024</v>
       </c>
-      <c r="G10">
-        <v>100</v>
-      </c>
       <c r="H10">
+        <v>100</v>
+      </c>
+      <c r="I10">
         <v>8025</v>
       </c>
-      <c r="I10">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11">
+      <c r="J10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11">
         <f t="shared" si="0"/>
         <v>9109</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>8025</v>
       </c>
-      <c r="C11">
-        <v>100</v>
-      </c>
       <c r="D11">
+        <v>100</v>
+      </c>
+      <c r="E11">
         <v>8024</v>
       </c>
-      <c r="E11">
-        <v>100</v>
-      </c>
       <c r="F11">
+        <v>100</v>
+      </c>
+      <c r="G11">
         <v>8023</v>
       </c>
-      <c r="G11">
-        <v>100</v>
-      </c>
       <c r="H11">
+        <v>100</v>
+      </c>
+      <c r="I11">
         <v>8022</v>
       </c>
-      <c r="I11">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12">
+      <c r="J11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B12">
+        <f t="shared" si="0"/>
         <v>9110</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>8026</v>
       </c>
-      <c r="C12">
+      <c r="D12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>9111</v>
+      </c>
+      <c r="C13">
+        <v>8027</v>
+      </c>
+      <c r="D13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>9112</v>
+      </c>
+      <c r="C14">
+        <v>8028</v>
+      </c>
+      <c r="D14">
+        <v>100</v>
+      </c>
+      <c r="E14">
+        <v>8029</v>
+      </c>
+      <c r="F14">
+        <v>100</v>
+      </c>
+      <c r="G14">
+        <v>8030</v>
+      </c>
+      <c r="H14">
+        <v>100</v>
+      </c>
+      <c r="I14">
+        <v>8031</v>
+      </c>
+      <c r="J14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>9113</v>
+      </c>
+      <c r="C15">
+        <v>8032</v>
+      </c>
+      <c r="D15">
+        <v>100</v>
+      </c>
+      <c r="E15">
+        <v>8033</v>
+      </c>
+      <c r="F15">
+        <v>100</v>
+      </c>
+      <c r="G15">
+        <v>8034</v>
+      </c>
+      <c r="H15">
+        <v>100</v>
+      </c>
+      <c r="I15">
+        <v>8035</v>
+      </c>
+      <c r="J15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>9114</v>
+      </c>
+      <c r="C16">
+        <v>8036</v>
+      </c>
+      <c r="D16">
+        <v>100</v>
+      </c>
+      <c r="E16">
+        <v>8037</v>
+      </c>
+      <c r="F16">
+        <v>100</v>
+      </c>
+      <c r="G16">
+        <v>8038</v>
+      </c>
+      <c r="H16">
+        <v>100</v>
+      </c>
+      <c r="I16">
+        <v>8039</v>
+      </c>
+      <c r="J16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>9115</v>
+      </c>
+      <c r="C17">
+        <v>8040</v>
+      </c>
+      <c r="D17">
+        <v>100</v>
+      </c>
+      <c r="E17">
+        <v>8041</v>
+      </c>
+      <c r="F17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>9116</v>
+      </c>
+      <c r="C18">
+        <v>8042</v>
+      </c>
+      <c r="D18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>9117</v>
+      </c>
+      <c r="C19">
+        <v>8043</v>
+      </c>
+      <c r="D19">
+        <v>100</v>
+      </c>
+      <c r="E19">
+        <v>8044</v>
+      </c>
+      <c r="F19">
+        <v>100</v>
+      </c>
+      <c r="G19">
+        <v>8045</v>
+      </c>
+      <c r="H19">
         <v>100</v>
       </c>
     </row>
@@ -1581,113 +2307,203 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{295686CE-12C7-44C8-8B10-67A78724A0F5}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
         <v>31</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B2">
         <v>9200</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>9100</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <f>A2+1</f>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <f>B2+1</f>
         <v>9201</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>9101</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <f t="shared" ref="A4:A9" si="0">A3+1</f>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <f t="shared" ref="B4:B8" si="0">B3+1</f>
         <v>9202</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>9102</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B5">
         <f t="shared" si="0"/>
         <v>9203</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>9103</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B6">
         <f t="shared" si="0"/>
         <v>9204</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>9104</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B7">
         <f t="shared" si="0"/>
         <v>9205</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>9105</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B8">
         <f t="shared" si="0"/>
         <v>9206</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>9106</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <f>A8+1</f>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B9">
+        <f>B8+1</f>
         <v>9207</v>
       </c>
-      <c r="B9">
-        <f t="shared" ref="B9:B11" si="1">B8+1</f>
+      <c r="C9">
+        <f t="shared" ref="C9" si="1">C8+1</f>
         <v>9107</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <f t="shared" ref="A10:A11" si="2">A9+1</f>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B10">
+        <f t="shared" ref="B10:B18" si="2">B9+1</f>
         <v>9208</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>9108</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>9109</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B11">
         <f t="shared" si="2"/>
         <v>9209</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>9110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="2"/>
+        <v>9210</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:C17" si="3">C11+1</f>
+        <v>9111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="2"/>
+        <v>9211</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="3"/>
+        <v>9112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="2"/>
+        <v>9212</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="3"/>
+        <v>9113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="2"/>
+        <v>9213</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="3"/>
+        <v>9114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="2"/>
+        <v>9214</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="3"/>
+        <v>9115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="2"/>
+        <v>9215</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="3"/>
+        <v>9116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="2"/>
+        <v>9216</v>
+      </c>
+      <c r="C18">
+        <v>9117</v>
       </c>
     </row>
   </sheetData>
@@ -1697,175 +2513,511 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F7636B0-73DA-492F-B863-BFF3740CF9D2}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="26.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B2">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>9200</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <f>A2+1</f>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <f>B2+1</f>
         <v>6</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>400</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>350</v>
       </c>
-      <c r="D3">
-        <f>D2+1</f>
+      <c r="E3">
+        <f>E2+1</f>
         <v>9201</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <f t="shared" ref="A4:A8" si="0">A3+1</f>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <f t="shared" ref="B4:B8" si="0">B3+1</f>
         <v>7</v>
-      </c>
-      <c r="B4">
-        <v>300</v>
       </c>
       <c r="C4">
         <v>300</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D11" si="1">D3+1</f>
+        <v>300</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E11" si="1">E3+1</f>
         <v>9202</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B5">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>200</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>250</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <f t="shared" si="1"/>
         <v>9203</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B6">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>150</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>350</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <f t="shared" si="1"/>
         <v>9204</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B7">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>150</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>200</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <f t="shared" si="1"/>
         <v>9205</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B8">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>200</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>350</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <f t="shared" si="1"/>
         <v>9206</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B9">
         <v>12</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>700</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>450</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <f t="shared" si="1"/>
         <v>9207</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B10">
         <v>13</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>150</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>50</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <f t="shared" si="1"/>
         <v>9208</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B11">
         <v>13</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>537</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>59</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <f t="shared" si="1"/>
         <v>9209</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12">
+        <v>30</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>9210</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13">
+        <v>17</v>
+      </c>
+      <c r="C13">
+        <v>120</v>
+      </c>
+      <c r="D13">
+        <v>70</v>
+      </c>
+      <c r="E13">
+        <v>9211</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14">
+        <v>17</v>
+      </c>
+      <c r="C14">
+        <v>65</v>
+      </c>
+      <c r="D14">
+        <v>1790</v>
+      </c>
+      <c r="E14">
+        <v>9211</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>74</v>
+      </c>
+      <c r="D15">
+        <v>1075</v>
+      </c>
+      <c r="E15">
+        <v>9211</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16">
+        <v>16</v>
+      </c>
+      <c r="C16">
+        <v>30</v>
+      </c>
+      <c r="D16">
+        <v>1583</v>
+      </c>
+      <c r="E16">
+        <v>9211</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>67</v>
+      </c>
+      <c r="D17">
+        <v>947</v>
+      </c>
+      <c r="E17">
+        <v>9211</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>200</v>
+      </c>
+      <c r="D18">
+        <v>1714</v>
+      </c>
+      <c r="E18">
+        <v>9212</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19">
+        <v>15</v>
+      </c>
+      <c r="C19">
+        <v>200</v>
+      </c>
+      <c r="D19">
+        <v>811</v>
+      </c>
+      <c r="E19">
+        <v>9212</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20">
+        <v>15</v>
+      </c>
+      <c r="C20">
+        <v>34</v>
+      </c>
+      <c r="D20">
+        <v>431</v>
+      </c>
+      <c r="E20">
+        <v>9212</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21">
+        <v>15</v>
+      </c>
+      <c r="C21">
+        <v>168</v>
+      </c>
+      <c r="D21">
+        <v>1199</v>
+      </c>
+      <c r="E21">
+        <v>9212</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22">
+        <v>16</v>
+      </c>
+      <c r="C22">
+        <v>52</v>
+      </c>
+      <c r="D22">
+        <v>333</v>
+      </c>
+      <c r="E22">
+        <v>9212</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23">
+        <v>17</v>
+      </c>
+      <c r="C23">
+        <v>120</v>
+      </c>
+      <c r="D23">
+        <v>89</v>
+      </c>
+      <c r="E23">
+        <v>9212</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24">
+        <v>16</v>
+      </c>
+      <c r="C24">
+        <v>200</v>
+      </c>
+      <c r="D24">
+        <v>1451</v>
+      </c>
+      <c r="E24">
+        <v>9212</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25">
+        <v>15</v>
+      </c>
+      <c r="C25">
+        <v>200</v>
+      </c>
+      <c r="D25">
+        <v>176</v>
+      </c>
+      <c r="E25">
+        <v>9213</v>
+      </c>
+      <c r="F25">
+        <v>30</v>
+      </c>
+      <c r="G25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26">
+        <v>9214</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27">
+        <v>9215</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28">
+        <v>21</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>9216</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29">
+        <v>18</v>
+      </c>
+      <c r="C29">
+        <v>69</v>
+      </c>
+      <c r="D29">
+        <v>1340</v>
+      </c>
+      <c r="E29">
+        <v>9211</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30">
+        <v>19</v>
+      </c>
+      <c r="C30">
+        <v>118</v>
+      </c>
+      <c r="D30">
+        <v>656</v>
+      </c>
+      <c r="E30">
+        <v>9211</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C31">
+        <v>45</v>
+      </c>
+      <c r="D31">
+        <v>628</v>
+      </c>
+      <c r="E31">
+        <v>9211</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C32">
+        <v>134</v>
+      </c>
+      <c r="D32">
+        <v>598</v>
+      </c>
+      <c r="E32">
+        <v>9211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>